<commit_message>
Added LR1, LR2, LR3
</commit_message>
<xml_diff>
--- a/LR3/111.xlsx
+++ b/LR3/111.xlsx
@@ -43,111 +43,9 @@
     <t>Штраф, руб</t>
   </si>
   <si>
-    <t>Адельвахаб</t>
-  </si>
-  <si>
-    <t>Алтынов</t>
-  </si>
-  <si>
-    <t>Альсайед</t>
-  </si>
-  <si>
-    <t>Асадуллин</t>
-  </si>
-  <si>
-    <t>Афанасьев</t>
-  </si>
-  <si>
-    <t>Бикмухаметов</t>
-  </si>
-  <si>
-    <t>Боровик</t>
-  </si>
-  <si>
-    <t>Галимов</t>
-  </si>
-  <si>
-    <t>Гиниатулин</t>
-  </si>
-  <si>
-    <t>Гюрбюз</t>
-  </si>
-  <si>
-    <t>Елеиссави</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ирканаев </t>
-  </si>
-  <si>
-    <t>Исмаел</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Калоша </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Макаров </t>
-  </si>
-  <si>
-    <t>Мухаметгалиев</t>
-  </si>
-  <si>
-    <t>Низамова</t>
-  </si>
-  <si>
-    <t>Озотюрк</t>
-  </si>
-  <si>
-    <t>Санутков</t>
-  </si>
-  <si>
-    <t>Сапожников</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сафиуллина </t>
-  </si>
-  <si>
-    <t>Стрижнев</t>
-  </si>
-  <si>
-    <t>Сулу</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Угурлуэл </t>
-  </si>
-  <si>
-    <t>Фазлиахметов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ханов </t>
-  </si>
-  <si>
-    <t>Хасаншина</t>
-  </si>
-  <si>
-    <t>Хассан</t>
-  </si>
-  <si>
-    <t>Шаабан</t>
-  </si>
-  <si>
-    <t>Шалаев</t>
-  </si>
-  <si>
-    <t>Шарафан</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Шафигуллина </t>
-  </si>
-  <si>
-    <t>Ершов</t>
-  </si>
-  <si>
     <t>Куропаткин 1</t>
   </si>
   <si>
-    <t>Куропаткин 3</t>
-  </si>
-  <si>
     <t>Куропаткин 2</t>
   </si>
   <si>
@@ -173,6 +71,108 @@
   </si>
   <si>
     <t>максимальная сумма к оплате, руб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Абделазиз </t>
+  </si>
+  <si>
+    <t xml:space="preserve">.Абдуллина </t>
+  </si>
+  <si>
+    <t>Акмалов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бабкин </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бахромов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Борисов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гафеев </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Городилова </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Девятов   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Исламов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Карманов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">КОканов  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">МохамедБоуйе </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Надеждин  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нуретдинов  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Павлова </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родионов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рудой </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Садыков </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Семагин </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Семенов  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Таухутдинов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фаляхутдинова </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Филатов  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хабк Осама </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хазипова </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хазов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хакимов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Халилов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хафизов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хрунин </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чепурченко  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ШабАнов </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шаймарданова </t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -552,22 +552,22 @@
         <v>5</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -575,18 +575,18 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2">
         <v>70</v>
       </c>
       <c r="D3" s="1">
-        <f>IF(A3&lt;=32,18.7,18.7/2)</f>
-        <v>18.7</v>
+        <f>IF(A3&lt;=32,$A$1*1.1,$A$1*0.55)</f>
+        <v>122.10000000000001</v>
       </c>
       <c r="E3" s="2">
         <f>C3*D3</f>
-        <v>1309</v>
+        <v>8547</v>
       </c>
       <c r="F3" s="4">
         <v>44813</v>
@@ -607,7 +607,7 @@
       </c>
       <c r="K3" s="3">
         <f>J3+E3</f>
-        <v>1309</v>
+        <v>8547</v>
       </c>
       <c r="L3" s="5"/>
     </row>
@@ -617,19 +617,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
         <f>C3-0.5</f>
         <v>69.5</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D38" si="0">IF(A4&lt;=32,18.7,18.7/2)</f>
-        <v>18.7</v>
+        <f t="shared" ref="D4:D38" si="0">IF(A4&lt;=32,$A$1*1.1,$A$1*0.55)</f>
+        <v>122.10000000000001</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E38" si="1">C4*D4</f>
-        <v>1299.6499999999999</v>
+        <v>8485.9500000000007</v>
       </c>
       <c r="F4" s="4">
         <v>44813</v>
@@ -650,7 +650,7 @@
       </c>
       <c r="K4" s="3">
         <f t="shared" ref="K4:K38" si="4">J4+E4</f>
-        <v>1299.6499999999999</v>
+        <v>8485.9500000000007</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C38" si="5">C4-0.5</f>
@@ -667,11 +667,11 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>1290.3</v>
+        <v>8424.9000000000015</v>
       </c>
       <c r="F5" s="4">
         <v>44813</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="K5" s="3">
         <f t="shared" si="4"/>
-        <v>1290.3</v>
+        <v>8424.9000000000015</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="5"/>
@@ -709,11 +709,11 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>1280.95</v>
+        <v>8363.85</v>
       </c>
       <c r="F6" s="4">
         <v>44813</v>
@@ -734,7 +734,7 @@
       </c>
       <c r="K6" s="3">
         <f t="shared" si="4"/>
-        <v>1280.95</v>
+        <v>8363.85</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="5"/>
@@ -751,11 +751,11 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>1271.5999999999999</v>
+        <v>8302.8000000000011</v>
       </c>
       <c r="F7" s="4">
         <v>44813</v>
@@ -776,7 +776,7 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="4"/>
-        <v>1271.5999999999999</v>
+        <v>8302.8000000000011</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -785,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="5"/>
@@ -793,11 +793,11 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>1262.25</v>
+        <v>8241.75</v>
       </c>
       <c r="F8" s="4">
         <v>44813</v>
@@ -818,7 +818,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" si="4"/>
-        <v>1262.25</v>
+        <v>8241.75</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="5"/>
@@ -835,11 +835,11 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>1252.8999999999999</v>
+        <v>8180.7000000000007</v>
       </c>
       <c r="F9" s="4">
         <v>44813</v>
@@ -860,7 +860,7 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="4"/>
-        <v>1252.8999999999999</v>
+        <v>8180.7000000000007</v>
       </c>
       <c r="L9" s="5"/>
     </row>
@@ -870,7 +870,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" si="5"/>
@@ -878,11 +878,11 @@
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>1243.55</v>
+        <v>8119.6500000000005</v>
       </c>
       <c r="F10" s="4">
         <v>44813</v>
@@ -903,7 +903,7 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="4"/>
-        <v>1243.55</v>
+        <v>8119.6500000000005</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" si="5"/>
@@ -920,11 +920,11 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
-        <v>1234.2</v>
+        <v>8058.6</v>
       </c>
       <c r="F11" s="4">
         <v>44813</v>
@@ -945,7 +945,7 @@
       </c>
       <c r="K11" s="3">
         <f t="shared" si="4"/>
-        <v>1234.2</v>
+        <v>8058.6</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="5"/>
@@ -962,11 +962,11 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>1224.8499999999999</v>
+        <v>7997.55</v>
       </c>
       <c r="F12" s="4">
         <v>44813</v>
@@ -987,7 +987,7 @@
       </c>
       <c r="K12" s="3">
         <f t="shared" si="4"/>
-        <v>1234.8499999999999</v>
+        <v>8007.55</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="5"/>
@@ -1004,11 +1004,11 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
-        <v>1215.5</v>
+        <v>7936.5000000000009</v>
       </c>
       <c r="F13" s="4">
         <v>44813</v>
@@ -1029,7 +1029,7 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="4"/>
-        <v>1235.5</v>
+        <v>7956.5000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="5"/>
@@ -1046,11 +1046,11 @@
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
-        <v>1206.1499999999999</v>
+        <v>7875.4500000000007</v>
       </c>
       <c r="F14" s="4">
         <v>44813</v>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="K14" s="3">
         <f t="shared" si="4"/>
-        <v>1236.1499999999999</v>
+        <v>7905.4500000000007</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1080,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="5"/>
@@ -1088,11 +1088,11 @@
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>1196.8</v>
+        <v>7814.4000000000005</v>
       </c>
       <c r="F15" s="4">
         <v>44813</v>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="4"/>
-        <v>1236.8</v>
+        <v>7854.4000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="5"/>
@@ -1130,11 +1130,11 @@
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>1187.45</v>
+        <v>7753.35</v>
       </c>
       <c r="F16" s="4">
         <v>44813</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="K16" s="3">
         <f t="shared" si="4"/>
-        <v>1237.45</v>
+        <v>7803.35</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1164,19 +1164,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2">
-        <f>C16-0.5</f>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>1178.0999999999999</v>
+        <v>7692.3</v>
       </c>
       <c r="F17" s="4">
         <v>44813</v>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="4"/>
-        <v>1238.0999999999999</v>
+        <v>7752.3</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1206,7 +1206,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" si="5"/>
@@ -1214,11 +1214,11 @@
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>1168.75</v>
+        <v>7631.2500000000009</v>
       </c>
       <c r="F18" s="4">
         <v>44813</v>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="4"/>
-        <v>1238.75</v>
+        <v>7701.2500000000009</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1248,7 +1248,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="5"/>
@@ -1256,11 +1256,11 @@
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>1159.3999999999999</v>
+        <v>7570.2000000000007</v>
       </c>
       <c r="F19" s="4">
         <v>44813</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="K19" s="3">
         <f t="shared" si="4"/>
-        <v>1239.3999999999999</v>
+        <v>7650.2000000000007</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="5"/>
@@ -1298,11 +1298,11 @@
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>1150.05</v>
+        <v>7509.1500000000005</v>
       </c>
       <c r="F20" s="4">
         <v>44813</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="K20" s="3">
         <f t="shared" si="4"/>
-        <v>1240.05</v>
+        <v>7599.1500000000005</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="5"/>
@@ -1340,11 +1340,11 @@
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>1140.7</v>
+        <v>7448.1</v>
       </c>
       <c r="F21" s="4">
         <v>44813</v>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="K21" s="3">
         <f t="shared" si="4"/>
-        <v>1240.7</v>
+        <v>7548.1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="5"/>
@@ -1382,11 +1382,11 @@
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="1"/>
-        <v>1131.3499999999999</v>
+        <v>7387.05</v>
       </c>
       <c r="F22" s="4">
         <v>44813</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="K22" s="3">
         <f t="shared" si="4"/>
-        <v>1241.3499999999999</v>
+        <v>7497.05</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="5"/>
@@ -1424,11 +1424,11 @@
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="1"/>
-        <v>1122</v>
+        <v>7326.0000000000009</v>
       </c>
       <c r="F23" s="4">
         <v>44813</v>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="K23" s="3">
         <f t="shared" si="4"/>
-        <v>1242</v>
+        <v>7446.0000000000009</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1458,7 +1458,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" si="5"/>
@@ -1466,11 +1466,11 @@
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="1"/>
-        <v>1112.6499999999999</v>
+        <v>7264.9500000000007</v>
       </c>
       <c r="F24" s="4">
         <v>44813</v>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="K24" s="3">
         <f t="shared" si="4"/>
-        <v>1242.6499999999999</v>
+        <v>7394.9500000000007</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" si="5"/>
@@ -1508,11 +1508,11 @@
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="1"/>
-        <v>1103.3</v>
+        <v>7203.9000000000005</v>
       </c>
       <c r="F25" s="4">
         <v>44813</v>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="K25" s="3">
         <f t="shared" si="4"/>
-        <v>1243.3</v>
+        <v>7343.9000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="5"/>
@@ -1550,11 +1550,11 @@
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="1"/>
-        <v>1093.95</v>
+        <v>7142.85</v>
       </c>
       <c r="F26" s="4">
         <v>44813</v>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="K26" s="3">
         <f t="shared" si="4"/>
-        <v>1243.95</v>
+        <v>7292.85</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="5"/>
@@ -1592,11 +1592,11 @@
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="1"/>
-        <v>1084.5999999999999</v>
+        <v>7081.8</v>
       </c>
       <c r="F27" s="4">
         <v>44813</v>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="K27" s="3">
         <f t="shared" si="4"/>
-        <v>1244.5999999999999</v>
+        <v>7241.8</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1626,7 +1626,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="5"/>
@@ -1634,11 +1634,11 @@
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="1"/>
-        <v>1075.25</v>
+        <v>7020.7500000000009</v>
       </c>
       <c r="F28" s="4">
         <v>44813</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="K28" s="3">
         <f t="shared" si="4"/>
-        <v>1245.25</v>
+        <v>7190.7500000000009</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="5"/>
@@ -1676,11 +1676,11 @@
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="1"/>
-        <v>1065.8999999999999</v>
+        <v>6959.7000000000007</v>
       </c>
       <c r="F29" s="4">
         <v>44813</v>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="K29" s="3">
         <f t="shared" si="4"/>
-        <v>1245.8999999999999</v>
+        <v>7139.7000000000007</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="5"/>
@@ -1718,11 +1718,11 @@
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="1"/>
-        <v>1056.55</v>
+        <v>6898.6500000000005</v>
       </c>
       <c r="F30" s="4">
         <v>44813</v>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="K30" s="3">
         <f t="shared" si="4"/>
-        <v>1246.55</v>
+        <v>7088.6500000000005</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C31" s="2">
         <f t="shared" si="5"/>
@@ -1760,11 +1760,11 @@
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="1"/>
-        <v>1047.2</v>
+        <v>6837.6</v>
       </c>
       <c r="F31" s="4">
         <v>44813</v>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="K31" s="3">
         <f t="shared" si="4"/>
-        <v>1247.2</v>
+        <v>7037.6</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,7 +1794,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" si="5"/>
@@ -1802,11 +1802,11 @@
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="1"/>
-        <v>1037.8499999999999</v>
+        <v>6776.55</v>
       </c>
       <c r="F32" s="4">
         <v>44813</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="K32" s="3">
         <f t="shared" si="4"/>
-        <v>1247.8499999999999</v>
+        <v>6986.55</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -1836,7 +1836,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C33" s="2">
         <f t="shared" si="5"/>
@@ -1844,11 +1844,11 @@
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="1"/>
-        <v>1028.5</v>
+        <v>6715.5000000000009</v>
       </c>
       <c r="F33" s="4">
         <v>44813</v>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="K33" s="3">
         <f t="shared" si="4"/>
-        <v>1248.5</v>
+        <v>6935.5000000000009</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2">
         <f t="shared" si="5"/>
@@ -1886,11 +1886,11 @@
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
-        <v>18.7</v>
+        <v>122.10000000000001</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="1"/>
-        <v>1019.15</v>
+        <v>6654.4500000000007</v>
       </c>
       <c r="F34" s="4">
         <v>44813</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="K34" s="3">
         <f t="shared" si="4"/>
-        <v>1249.1500000000001</v>
+        <v>6884.4500000000007</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C35" s="2">
         <f t="shared" si="5"/>
@@ -1928,11 +1928,11 @@
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
-        <v>9.35</v>
+        <v>61.050000000000004</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="1"/>
-        <v>504.9</v>
+        <v>3296.7000000000003</v>
       </c>
       <c r="F35" s="4">
         <v>44813</v>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" si="4"/>
-        <v>744.9</v>
+        <v>3536.7000000000003</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C36" s="2">
         <f t="shared" si="5"/>
@@ -1970,11 +1970,11 @@
       </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
-        <v>9.35</v>
+        <v>61.050000000000004</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="1"/>
-        <v>500.22499999999997</v>
+        <v>3266.1750000000002</v>
       </c>
       <c r="F36" s="4">
         <v>44813</v>
@@ -1995,7 +1995,7 @@
       </c>
       <c r="K36" s="3">
         <f t="shared" si="4"/>
-        <v>750.22499999999991</v>
+        <v>3516.1750000000002</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" si="5"/>
@@ -2012,11 +2012,11 @@
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
-        <v>9.35</v>
+        <v>61.050000000000004</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="1"/>
-        <v>495.54999999999995</v>
+        <v>3235.65</v>
       </c>
       <c r="F37" s="4">
         <v>44813</v>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="K37" s="3">
         <f t="shared" si="4"/>
-        <v>755.55</v>
+        <v>3495.65</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -2046,7 +2046,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C38" s="2">
         <f t="shared" si="5"/>
@@ -2054,11 +2054,11 @@
       </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
-        <v>9.35</v>
+        <v>61.050000000000004</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="1"/>
-        <v>490.875</v>
+        <v>3205.125</v>
       </c>
       <c r="F38" s="4">
         <v>44813</v>
@@ -2079,21 +2079,21 @@
       </c>
       <c r="K38" s="3">
         <f t="shared" si="4"/>
-        <v>760.875</v>
+        <v>3475.125</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="C40" s="5">
         <f>SUM(K3:K38)</f>
-        <v>43021.950000000004</v>
+        <v>260006.85</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C41" s="2">
         <f>AVERAGE(C3:C38)</f>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="C42" s="2">
         <f>MAX(H3:H38)</f>
@@ -2111,11 +2111,11 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C43" s="3">
         <f>MAX(K3:K38)</f>
-        <v>1309</v>
+        <v>8547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>